<commit_message>
DEV3.1 - Enquiry Management
</commit_message>
<xml_diff>
--- a/resources/data/ProjectEnquiry.xlsx
+++ b/resources/data/ProjectEnquiry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Desktop/NTU/NTU_Y1S2/SC2002/Assignment/BTO_Application/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47DAFDC9-5A73-45E6-B73F-8CFF7844F1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B8113E-C9CD-4347-9D01-97614C414291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{A3D7CCAD-0F3E-41F5-B920-33C4AF4440B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A3D7CCAD-0F3E-41F5-B920-33C4AF4440B4}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectEnquiry" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NRIC</t>
+  </si>
+  <si>
+    <t>PROJECT ID</t>
+  </si>
+  <si>
+    <t>ENQUIRY</t>
+  </si>
+  <si>
+    <t>REPLY</t>
+  </si>
+  <si>
+    <t>ENQUIRY_DATE</t>
+  </si>
+  <si>
+    <t>REPLY_DATE</t>
+  </si>
+  <si>
+    <t>S1234567A</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>T7654321B</t>
+  </si>
+  <si>
+    <t>Hello to You!</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,8 +537,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -875,12 +915,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806557D-9436-4A10-9BD6-85E3C8C8CAFC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.83203125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.83203125" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.6640625" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45764.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>45764.81342239583</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45764</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DEV 5 - CLI Changes for Manager Project and Enquiry
</commit_message>
<xml_diff>
--- a/resources/data/ProjectEnquiry.xlsx
+++ b/resources/data/ProjectEnquiry.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>hello how do i do this</t>
+  </si>
+  <si>
+    <t>hello hello</t>
   </si>
 </sst>
 </file>
@@ -611,9 +614,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -1081,13 +1085,13 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="n" s="7">
+        <v>35</v>
+      </c>
+      <c r="F3" t="n" s="23">
         <v>45764.0</v>
       </c>
-      <c r="G3" t="n" s="7">
-        <v>45767.87215314815</v>
+      <c r="G3" t="n" s="23">
+        <v>45769.925410208336</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
MVC formatted for OFFICER and APPLICANTs
</commit_message>
<xml_diff>
--- a/resources/data/ProjectEnquiry.xlsx
+++ b/resources/data/ProjectEnquiry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3695EE-5FE3-6947-AE5B-92F44085647A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0B3695EE-5FE3-6947-AE5B-92F44085647A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ABA3BC8-DCF2-492A-BD72-074202D7595E}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{A3D7CCAD-0F3E-41F5-B920-33C4AF4440B4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{A3D7CCAD-0F3E-41F5-B920-33C4AF4440B4}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectEnquiry" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>S9876543C</t>
+  </si>
+  <si>
+    <t>falllll</t>
+  </si>
+  <si>
+    <t>testttt</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -537,9 +549,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -919,21 +934,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806557D-9436-4A10-9BD6-85E3C8C8CAFC}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="A2:G12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.46484375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -956,96 +971,84 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G2" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45770.229960462966</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>45770.315135497687</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45770.318008113427</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="n" s="8">
+        <v>45770.60340975694</v>
+      </c>
+      <c r="G4" t="n" s="8">
+        <v>45770.65246978009</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="n" s="2">
-        <v>45770.229960462966</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="n" s="4">
-        <v>45770.31513549769</v>
-      </c>
-      <c r="G14" t="n" s="4">
-        <v>45770.31800811343</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="n" s="5">
-        <v>45770.53296790509</v>
+      <c r="F5" t="n" s="4">
+        <v>45770.63536047454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>